<commit_message>
did some work on mixed optimiser
</commit_message>
<xml_diff>
--- a/results/60s_5d_Polar_iainDesktop_M8_D9_H9_min4/Alt_scheduleraw_up_to_shift 200.xlsx
+++ b/results/60s_5d_Polar_iainDesktop_M8_D9_H9_min4/Alt_scheduleraw_up_to_shift 200.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fe753deea9fa81e/Documents/GitHub/Strathdar/results/60s_5d_Polar_iainDesktop_M8_D9_H9_min4/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_4C2FC68DA6662BB7BF372F90FC2D62B140B5DE34" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D446B002-9F42-470A-99A6-E159E647AE00}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="she7et1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -46,8 +52,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +116,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -156,7 +170,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -188,9 +202,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,6 +254,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -397,14 +447,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="J99" sqref="J99"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +485,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -465,7 +517,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -497,7 +549,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -529,7 +581,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -561,7 +613,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -593,7 +645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -625,7 +677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -657,7 +709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -689,7 +741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -721,7 +773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -753,7 +805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -785,7 +837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -817,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -849,7 +901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -881,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -913,7 +965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -945,7 +997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -977,7 +1029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1009,7 +1061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1041,7 +1093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1073,7 +1125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1105,7 +1157,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1137,7 +1189,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1169,7 +1221,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1201,7 +1253,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1233,7 +1285,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1265,7 +1317,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1297,7 +1349,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1329,7 +1381,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1361,7 +1413,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1393,7 +1445,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1425,7 +1477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1457,7 +1509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1489,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1521,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1553,7 +1605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1585,7 +1637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1617,7 +1669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1649,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1681,7 +1733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1713,7 +1765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1745,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1777,7 +1829,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1809,7 +1861,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1841,7 +1893,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1873,7 +1925,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1905,7 +1957,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1937,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1969,7 +2021,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2001,7 +2053,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2033,7 +2085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2065,7 +2117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2097,7 +2149,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2129,7 +2181,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2161,7 +2213,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2193,7 +2245,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2225,7 +2277,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2257,7 +2309,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2289,7 +2341,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2321,7 +2373,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2353,7 +2405,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2385,7 +2437,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2417,7 +2469,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2449,7 +2501,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2481,7 +2533,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2513,7 +2565,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2545,7 +2597,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2577,7 +2629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2609,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2641,7 +2693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2673,7 +2725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2705,7 +2757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2737,7 +2789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2769,7 +2821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2801,7 +2853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2833,7 +2885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2865,7 +2917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2897,7 +2949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2929,7 +2981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2961,7 +3013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2993,7 +3045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -3025,7 +3077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -3057,7 +3109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -3089,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -3121,7 +3173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3153,7 +3205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3185,7 +3237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3217,7 +3269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3249,7 +3301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3281,7 +3333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3313,7 +3365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3345,7 +3397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3377,7 +3429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -3409,7 +3461,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -3441,7 +3493,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3473,7 +3525,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -3505,7 +3557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -3537,7 +3589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -3569,7 +3621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -3598,10 +3650,10 @@
         <v>34650684</v>
       </c>
       <c r="J100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -3630,10 +3682,10 @@
         <v>34650684</v>
       </c>
       <c r="J101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -3662,10 +3714,10 @@
         <v>34560864</v>
       </c>
       <c r="J102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -3694,10 +3746,10 @@
         <v>34471044</v>
       </c>
       <c r="J103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -3726,10 +3778,10 @@
         <v>34381224</v>
       </c>
       <c r="J104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -3761,7 +3813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -3793,7 +3845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -3825,7 +3877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -3857,7 +3909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -3889,7 +3941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -3921,7 +3973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -3953,7 +4005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -3985,7 +4037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -4017,7 +4069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -4049,7 +4101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -4081,7 +4133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -4113,7 +4165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -4145,7 +4197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -4177,7 +4229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -4209,7 +4261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -4241,7 +4293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -4273,7 +4325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -4305,7 +4357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -4337,7 +4389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -4369,7 +4421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -4401,7 +4453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -4433,7 +4485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -4465,7 +4517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -4497,7 +4549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -4529,7 +4581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -4561,7 +4613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -4593,7 +4645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -4625,7 +4677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -4657,7 +4709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -4689,7 +4741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -4721,7 +4773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -4753,7 +4805,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -4785,7 +4837,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -4817,7 +4869,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -4849,7 +4901,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -4881,7 +4933,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -4913,7 +4965,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -4945,7 +4997,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -4977,7 +5029,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -5009,7 +5061,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -5041,7 +5093,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -5073,7 +5125,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -5105,7 +5157,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -5137,7 +5189,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -5169,7 +5221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -5201,7 +5253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -5233,7 +5285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -5265,7 +5317,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -5297,7 +5349,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -5329,7 +5381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -5361,7 +5413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -5393,7 +5445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -5425,7 +5477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -5457,7 +5509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -5489,7 +5541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -5521,7 +5573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -5553,7 +5605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -5585,7 +5637,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -5617,7 +5669,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -5649,7 +5701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -5681,7 +5733,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -5713,7 +5765,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -5745,7 +5797,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -5777,7 +5829,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -5809,7 +5861,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -5841,7 +5893,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -5873,7 +5925,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -5905,7 +5957,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -5937,7 +5989,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -5969,7 +6021,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -6001,7 +6053,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -6033,7 +6085,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -6065,7 +6117,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -6097,7 +6149,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -6129,7 +6181,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -6161,7 +6213,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -6193,7 +6245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -6225,7 +6277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -6257,7 +6309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -6289,7 +6341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -6321,7 +6373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -6353,7 +6405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -6385,7 +6437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -6417,7 +6469,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -6449,7 +6501,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -6481,7 +6533,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -6513,7 +6565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -6545,7 +6597,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -6577,7 +6629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -6609,7 +6661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -6641,7 +6693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -6673,7 +6725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -6705,7 +6757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -6737,7 +6789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -6769,7 +6821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -6801,7 +6853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>199</v>
       </c>

</xml_diff>